<commit_message>
FB001-23: Install the React TypeScript project
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1290AC38-F0F9-4D40-AC0D-FCEE1CE8D189}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90690415-488F-5340-B85A-A0F351556BF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="2860" windowWidth="36340" windowHeight="17620" activeTab="1" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="460" yWindow="1200" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
-    <sheet name="SCRUM-1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="FB001-1" sheetId="2" r:id="rId2"/>
+    <sheet name="FB001-15" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -38,16 +38,10 @@
     <t xml:space="preserve">This is the foundation for the entire application, including some necessary features like authentication, building the common Library, EF core base setup, Dockerize service, Manage Development Environment by Docker compose, Setting up API Testing, Preparing Kubernetes Environment, CI/CD </t>
   </si>
   <si>
-    <t>SCRUM-1</t>
-  </si>
-  <si>
     <t>Implement User Relationship Features</t>
   </si>
   <si>
     <t>The context of this epic is to build page, so user to be able to access to the own profile page, and can make request to create a relationship with anyone</t>
-  </si>
-  <si>
-    <t>SCRUM-2</t>
   </si>
   <si>
     <t>Epic Id</t>
@@ -185,13 +179,142 @@
   </si>
   <si>
     <t>SCRUM-14</t>
+  </si>
+  <si>
+    <t>Implement the UI Service by React TypeScript</t>
+  </si>
+  <si>
+    <t>Build the core UI Service by using ReactTS, using Redux Zero to manage State more effectively, containerizing the application to Images, building CI/CD for the FE service to deploy the Staging and Production environment</t>
+  </si>
+  <si>
+    <t>FB001-1</t>
+  </si>
+  <si>
+    <t>FB001-2</t>
+  </si>
+  <si>
+    <t>FB001-15</t>
+  </si>
+  <si>
+    <t>Setup UI and Install Packages, Clean Code</t>
+  </si>
+  <si>
+    <t>Setup UI project and install some necessary Packages</t>
+  </si>
+  <si>
+    <t>Create Login Page</t>
+  </si>
+  <si>
+    <t>Clean Code</t>
+  </si>
+  <si>
+    <t>UAM for user based on Role base</t>
+  </si>
+  <si>
+    <t>Containerize the application</t>
+  </si>
+  <si>
+    <t>Containerize the UI application to the images and run it by using Docker Compose</t>
+  </si>
+  <si>
+    <t>Create CI/CD to deploy to Cluster for two environments</t>
+  </si>
+  <si>
+    <t>Create Jenkins Job to automate deployment for UI project</t>
+  </si>
+  <si>
+    <t>Create User Access Management to allow user access to the page based on their Rolex, and define some basic Account, Role</t>
+  </si>
+  <si>
+    <t>Error handling</t>
+  </si>
+  <si>
+    <t>Install the first UI project</t>
+  </si>
+  <si>
+    <t>Setup Hook</t>
+  </si>
+  <si>
+    <t>Install and setip basic Redux Zero</t>
+  </si>
+  <si>
+    <t>Setup Redux Zero</t>
+  </si>
+  <si>
+    <t>Install and setip basic Hook</t>
+  </si>
+  <si>
+    <t>Update User service to support Role Base communication</t>
+  </si>
+  <si>
+    <t>UAM routing on UI</t>
+  </si>
+  <si>
+    <t>Setup Middleware by using Redux-saga</t>
+  </si>
+  <si>
+    <t>Install and setup basic middleware by using Redux-saga</t>
+  </si>
+  <si>
+    <t>Update User service and Database to support Role Base access to the application, and define some fixed Account, Role (Admin, User, Guest) by script</t>
+  </si>
+  <si>
+    <t>Set up UI project and install some necessary Packages, set up Redux Zero to manage state and hooks. Redux-saga</t>
+  </si>
+  <si>
+    <t>SCRUM-16</t>
+  </si>
+  <si>
+    <t>SCRUM-17</t>
+  </si>
+  <si>
+    <t>Create login page to Interact with User service API to indicate whether this use is authenticated or not, using localStorage to store the JWT token</t>
+  </si>
+  <si>
+    <t>SCRUM-18</t>
+  </si>
+  <si>
+    <t>SCRUM-19</t>
+  </si>
+  <si>
+    <t>SCRUM-20</t>
+  </si>
+  <si>
+    <t>Routing the user to the Error page when they face an error</t>
+  </si>
+  <si>
+    <t>SCRUM-21</t>
+  </si>
+  <si>
+    <t>SCRUM-22</t>
+  </si>
+  <si>
+    <t>SCRUM-23</t>
+  </si>
+  <si>
+    <t>SCRUM-24</t>
+  </si>
+  <si>
+    <t>SCRUM-25</t>
+  </si>
+  <si>
+    <t>SCRUM-26</t>
+  </si>
+  <si>
+    <t>SCRUM-27</t>
+  </si>
+  <si>
+    <t>SCRUM-28</t>
+  </si>
+  <si>
+    <t>Create the UI to be able to access the acceptable page based on their role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,8 +360,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,8 +399,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,12 +509,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -408,21 +561,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -438,6 +579,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -456,13 +606,45 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,6 +803,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDEBF7"/>
+      <color rgb="FFFFF2CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -944,7 +1132,7 @@
   <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -957,18 +1145,18 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>3</v>
+      <c r="A3" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>1</v>
@@ -978,22 +1166,26 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="62" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>6</v>
+      <c r="A4" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="50" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
@@ -1032,12 +1224,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{BD44C65E-8536-A141-803F-7CE5EE80C51F}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{F7ECB6ED-6164-D842-BBE6-0F5FDE49F903}"/>
+    <hyperlink ref="A3" r:id="rId1" display="SCRUM-1" xr:uid="{BD44C65E-8536-A141-803F-7CE5EE80C51F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1046,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71808AEC-1F3F-6046-97A2-6661A8254E1D}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,232 +1253,232 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="14" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A6" s="21"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="19" t="s">
+      <c r="C9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="19" t="s">
+      <c r="E10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="E11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="20" t="s">
+      <c r="C12" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="20" t="s">
+      <c r="E12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A13" s="25"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="E13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
@@ -1323,6 +1514,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -1330,9 +1524,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1341,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:F26"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1358,161 +1549,237 @@
     <col min="7" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+    <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+    </row>
+    <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A6" s="37"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A7" s="37"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+    </row>
+    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
@@ -1539,15 +1806,33 @@
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FB001-29: Create a Login page, Layout for Admin and Member, create basic Permission base routing on UI
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90690415-488F-5340-B85A-A0F351556BF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3780CE2-133D-3A4C-9F55-1473963DAF8E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="1200" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>Description</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Create the UI to be able to access the acceptable page based on their role</t>
+  </si>
+  <si>
+    <t>SCRUM-29</t>
+  </si>
+  <si>
+    <t>Create a Login UI page with Role base routing</t>
+  </si>
+  <si>
+    <t>Create the first Login page with the necessary animation by using react. Permission base basic for routing the user, Create AdminLayout and MemberLayout and permission needed for routing</t>
   </si>
 </sst>
 </file>
@@ -579,36 +588,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -635,6 +614,39 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -643,9 +655,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1253,12 +1262,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1281,13 +1290,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="36" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1301,9 +1310,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="20"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1315,9 +1324,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1329,7 +1338,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -1357,13 +1366,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1377,9 +1386,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1391,13 +1400,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1411,9 +1420,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1532,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
-  <dimension ref="A2:F26"/>
+  <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C5" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,12 +1559,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1578,168 +1587,174 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="36" t="s">
+    <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
+      <c r="A6" s="27"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F7" s="19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A9" s="28"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E9" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F9" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C10" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-    </row>
-    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C11" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-    </row>
-    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B12" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C12" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-    </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C13" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D13" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E13" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F13" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+    <row r="14" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B14" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C14" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D14" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F14" s="22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
@@ -1822,17 +1837,25 @@
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="C5:C9"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FB001-17: Change the port 6000 to safety port 4000
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3780CE2-133D-3A4C-9F55-1473963DAF8E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09147EBD-E52D-F44B-93BD-5A895CC33F92}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="1200" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
@@ -232,36 +232,15 @@
     <t>Install the first UI project</t>
   </si>
   <si>
-    <t>Setup Hook</t>
-  </si>
-  <si>
-    <t>Install and setip basic Redux Zero</t>
-  </si>
-  <si>
-    <t>Setup Redux Zero</t>
-  </si>
-  <si>
-    <t>Install and setip basic Hook</t>
-  </si>
-  <si>
     <t>Update User service to support Role Base communication</t>
   </si>
   <si>
     <t>UAM routing on UI</t>
   </si>
   <si>
-    <t>Setup Middleware by using Redux-saga</t>
-  </si>
-  <si>
-    <t>Install and setup basic middleware by using Redux-saga</t>
-  </si>
-  <si>
     <t>Update User service and Database to support Role Base access to the application, and define some fixed Account, Role (Admin, User, Guest) by script</t>
   </si>
   <si>
-    <t>Set up UI project and install some necessary Packages, set up Redux Zero to manage state and hooks. Redux-saga</t>
-  </si>
-  <si>
     <t>SCRUM-16</t>
   </si>
   <si>
@@ -317,6 +296,27 @@
   </si>
   <si>
     <t>Create the first Login page with the necessary animation by using react. Permission base basic for routing the user, Create AdminLayout and MemberLayout and permission needed for routing</t>
+  </si>
+  <si>
+    <t>Setup Redux</t>
+  </si>
+  <si>
+    <t>Install and setip basic Redux</t>
+  </si>
+  <si>
+    <t>Research React Hook</t>
+  </si>
+  <si>
+    <t>Research the hook basic and advance</t>
+  </si>
+  <si>
+    <t>Setup Middleware by using Redux-Thunk</t>
+  </si>
+  <si>
+    <t>Install and setup basic middleware by using Redux-Thunk</t>
+  </si>
+  <si>
+    <t>Set up UI project and install some necessary Packages, set up Redux to manage state and hooks. Redux-Thunk</t>
   </si>
 </sst>
 </file>
@@ -1544,7 +1544,7 @@
   <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1588,16 +1588,16 @@
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>65</v>
@@ -1611,13 +1611,13 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="26" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
@@ -1625,13 +1625,13 @@
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="26" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
@@ -1639,13 +1639,13 @@
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="26" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
@@ -1653,24 +1653,24 @@
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
       <c r="D9" s="26" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>59</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>61</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>58</v>
@@ -1715,38 +1715,38 @@
         <v>63</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
FB001-23: Recreate Angular Typescript Project
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09147EBD-E52D-F44B-93BD-5A895CC33F92}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B6910D-3A44-764A-BE8E-8B4AEE4B0351}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="1200" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="440" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
   <si>
     <t>Description</t>
   </si>
@@ -295,28 +295,31 @@
     <t>Create a Login UI page with Role base routing</t>
   </si>
   <si>
-    <t>Create the first Login page with the necessary animation by using react. Permission base basic for routing the user, Create AdminLayout and MemberLayout and permission needed for routing</t>
-  </si>
-  <si>
-    <t>Setup Redux</t>
-  </si>
-  <si>
-    <t>Install and setip basic Redux</t>
-  </si>
-  <si>
-    <t>Research React Hook</t>
-  </si>
-  <si>
     <t>Research the hook basic and advance</t>
   </si>
   <si>
-    <t>Setup Middleware by using Redux-Thunk</t>
-  </si>
-  <si>
-    <t>Install and setup basic middleware by using Redux-Thunk</t>
-  </si>
-  <si>
-    <t>Set up UI project and install some necessary Packages, set up Redux to manage state and hooks. Redux-Thunk</t>
+    <t>Set up UI project and install some necessary Packages, set up NgRx to manage global state</t>
+  </si>
+  <si>
+    <t>Create the first Login page with the necessary animation by using react Check Mark. Permission base basic for routing the user Check Mark. Create AdminLayout and MemberLayout and permission needed for routing Check Mark</t>
+  </si>
+  <si>
+    <t>Setup NgRx</t>
+  </si>
+  <si>
+    <t>Install and setip basic NgRx</t>
+  </si>
+  <si>
+    <t>Research React Hook (descope)</t>
+  </si>
+  <si>
+    <t>Setup Middleware</t>
+  </si>
+  <si>
+    <t>Install and setup basic middleware</t>
+  </si>
+  <si>
+    <t>Create the first Login page with the necessary animation by using angular. Permission base basic for routing the user, Create AdminLayout and MemberLayout and permission needed for routing</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -616,6 +619,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1262,12 +1271,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1290,13 +1299,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="38" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1310,9 +1319,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1324,9 +1333,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1366,13 +1375,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1386,9 +1395,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1400,13 +1409,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="34" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1420,9 +1429,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1541,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
-  <dimension ref="A2:F27"/>
+  <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1559,12 +1568,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1587,16 +1596,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="26" t="s">
+      <c r="C5" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>78</v>
       </c>
       <c r="E5" s="19" t="s">
@@ -1608,161 +1617,167 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>86</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="26" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>91</v>
+      <c r="E8" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="26" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="100" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B11" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C11" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B12" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C13" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B14" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C14" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D14" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+    <row r="15" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B15" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D15" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E15" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F15" s="22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+    <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B16" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
@@ -1845,12 +1860,20 @@
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
FB001-30: Support multiple environments while running and building
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B6910D-3A44-764A-BE8E-8B4AEE4B0351}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F187A5-0AEC-E74C-9FA3-F051F0284871}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="99">
   <si>
     <t>Description</t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>Create the first Login page with the necessary animation by using angular. Permission base basic for routing the user, Create AdminLayout and MemberLayout and permission needed for routing</t>
+  </si>
+  <si>
+    <t>Suport Multiple Environment</t>
+  </si>
+  <si>
+    <t>Create an environment file to support multiple environments</t>
+  </si>
+  <si>
+    <t>SCRUM-30</t>
   </si>
 </sst>
 </file>
@@ -537,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,7 +615,6 @@
     <xf numFmtId="49" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1271,12 +1279,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1299,13 +1307,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1319,9 +1327,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1333,9 +1341,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1375,13 +1383,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1395,9 +1403,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1409,13 +1417,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1429,9 +1437,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1553,7 +1561,7 @@
   <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C5" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1568,12 +1576,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1599,10 +1607,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1616,9 +1624,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1630,9 +1638,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1644,23 +1652,23 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="29" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -1672,16 +1680,16 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="100" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="29" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1723,9 +1731,15 @@
       <c r="C13" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="D13" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
@@ -1737,7 +1751,7 @@
       <c r="C14" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>82</v>
       </c>
       <c r="E14" s="19" t="s">
@@ -1757,7 +1771,7 @@
       <c r="C15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>83</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -1774,7 +1788,7 @@
       <c r="B16" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>

</xml_diff>

<commit_message>
FB001-35: Containerize the IdP API Server application
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F187A5-0AEC-E74C-9FA3-F051F0284871}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6155E-4853-144F-AAE1-B42A5674F1A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="420" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="3" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
     <sheet name="FB001-1" sheetId="2" r:id="rId2"/>
     <sheet name="FB001-15" sheetId="4" r:id="rId3"/>
+    <sheet name="FB001-31" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="118">
   <si>
     <t>Description</t>
   </si>
@@ -329,6 +330,63 @@
   </si>
   <si>
     <t>SCRUM-30</t>
+  </si>
+  <si>
+    <t>Implement IdP Server for Authentication</t>
+  </si>
+  <si>
+    <t>SCRUM-32</t>
+  </si>
+  <si>
+    <t>Create Dotnet API Server for IdP Server</t>
+  </si>
+  <si>
+    <t>SCRUM-33</t>
+  </si>
+  <si>
+    <t>SCRUM-34</t>
+  </si>
+  <si>
+    <t>SCRUM-35</t>
+  </si>
+  <si>
+    <t>SCRUM-36</t>
+  </si>
+  <si>
+    <t>SCRUM-37</t>
+  </si>
+  <si>
+    <t>SCRUM-38</t>
+  </si>
+  <si>
+    <t>SCRUM-39</t>
+  </si>
+  <si>
+    <t>Implement the first basic IdP server without database designation</t>
+  </si>
+  <si>
+    <t>Create a login page to Interact with the IdP Server</t>
+  </si>
+  <si>
+    <t>Create first Dotnet API server within the first login endpoint</t>
+  </si>
+  <si>
+    <t>Implement the basic API Server within the basic login endpoint without database</t>
+  </si>
+  <si>
+    <t>Containerize the IdP API Server application</t>
+  </si>
+  <si>
+    <t>Create CI/CD to deploy IdP API to Cluster for two environments</t>
+  </si>
+  <si>
+    <t>Create the first angular application by integrating the login API endpoint</t>
+  </si>
+  <si>
+    <t>Containerize the IdP UI application</t>
+  </si>
+  <si>
+    <t>Create CI/CD to deploy IdP UI to Cluster for two environments</t>
   </si>
 </sst>
 </file>
@@ -546,7 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -634,6 +692,9 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -672,6 +733,42 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1279,12 +1376,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1307,13 +1404,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="38" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1327,9 +1424,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1341,9 +1438,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1383,13 +1480,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1403,9 +1500,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1417,13 +1514,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1437,9 +1534,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1560,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C9"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1576,12 +1673,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1607,10 +1704,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="42" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1625,8 +1722,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1639,8 +1736,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1653,8 +1750,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -1667,8 +1764,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -1897,4 +1994,281 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B875EC8-ACE7-474A-B26E-31D1589A2243}">
+  <dimension ref="A2:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="61.5" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="74.83203125" customWidth="1"/>
+    <col min="6" max="6" width="80.5" customWidth="1"/>
+    <col min="7" max="9" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A6" s="46"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A7" s="47"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A8" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A9" s="49"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A10" s="50"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+    </row>
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FB001-37: Create the first angular application by integrating the login API endpoint
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6155E-4853-144F-AAE1-B42A5674F1A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0502CFC0-0F3A-514B-A9CE-B4B621E2C1B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="3" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="420" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
   <si>
     <t>Description</t>
   </si>
@@ -387,6 +387,15 @@
   </si>
   <si>
     <t>Create CI/CD to deploy IdP UI to Cluster for two environments</t>
+  </si>
+  <si>
+    <t>Internal Login With IdP server</t>
+  </si>
+  <si>
+    <t>Implement the feature for Internal User Login with IdP server</t>
+  </si>
+  <si>
+    <t>SCRUM-40</t>
   </si>
 </sst>
 </file>
@@ -1657,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1890,13 +1899,19 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
     </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+    <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
@@ -2000,7 +2015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B875EC8-ACE7-474A-B26E-31D1589A2243}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FB001-41,42,43: Login within server permission, Internal user login via IdP, Exchange IdP token to new token
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0502CFC0-0F3A-514B-A9CE-B4B621E2C1B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70933857-999A-3C44-8BC3-51E658E2DF0D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1300" windowWidth="37820" windowHeight="19660" activeTab="2" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="3" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>Description</t>
   </si>
@@ -396,13 +396,37 @@
   </si>
   <si>
     <t>SCRUM-40</t>
+  </si>
+  <si>
+    <t>SCRUM-41</t>
+  </si>
+  <si>
+    <t>SCRUM-42</t>
+  </si>
+  <si>
+    <t>Implement Internal User Login</t>
+  </si>
+  <si>
+    <t>Implement Temporary API to Exchange the new token from IdP token</t>
+  </si>
+  <si>
+    <t>[Temporary] Implement API to Exchange IdP token</t>
+  </si>
+  <si>
+    <t>SCRUM-43</t>
+  </si>
+  <si>
+    <t>[Temporary] Implement API to get User Permissions from token</t>
+  </si>
+  <si>
+    <t>Implement Temporary API to get some fake permissions to support the IdP External Login feature</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,8 +479,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +529,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -613,7 +651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -704,6 +742,9 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -743,6 +784,18 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -752,24 +805,12 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -778,6 +819,12 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1385,12 +1432,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1413,13 +1460,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1433,9 +1480,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1447,9 +1494,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1489,13 +1536,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1509,9 +1556,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1523,13 +1570,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1543,9 +1590,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1664,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
-  <dimension ref="A2:F28"/>
+  <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1682,12 +1729,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1713,10 +1760,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="43" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1731,8 +1778,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1745,8 +1792,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1759,8 +1806,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -1773,8 +1820,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -1900,34 +1947,52 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="D17" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
@@ -1994,18 +2059,29 @@
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2015,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B875EC8-ACE7-474A-B26E-31D1589A2243}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2031,12 +2107,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2059,13 +2135,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="43" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2079,9 +2155,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2093,9 +2169,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2107,13 +2183,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="55" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2127,9 +2203,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="55"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2141,9 +2217,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="50"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
FB001-47: Create the first Ocelot service and forward request
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70933857-999A-3C44-8BC3-51E658E2DF0D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5074F2-E380-EB4B-9DF1-71461067B484}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="3" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="4" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
     <sheet name="FB001-1" sheetId="2" r:id="rId2"/>
     <sheet name="FB001-15" sheetId="4" r:id="rId3"/>
     <sheet name="FB001-31" sheetId="5" r:id="rId4"/>
+    <sheet name="FB001-44" sheetId="6" r:id="rId5"/>
+    <sheet name="FB001-50" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="154">
   <si>
     <t>Description</t>
   </si>
@@ -420,6 +422,81 @@
   </si>
   <si>
     <t>Implement Temporary API to get some fake permissions to support the IdP External Login feature</t>
+  </si>
+  <si>
+    <t>Implement Ocelot Service as API Gateway</t>
+  </si>
+  <si>
+    <t>Implement the basic Ocelot service</t>
+  </si>
+  <si>
+    <t>SCRUM-45</t>
+  </si>
+  <si>
+    <t>SCRUM-46</t>
+  </si>
+  <si>
+    <t>SCRUM-47</t>
+  </si>
+  <si>
+    <t>SCRUM-48</t>
+  </si>
+  <si>
+    <t>Create the first Ocelot service and forward request</t>
+  </si>
+  <si>
+    <t>Integrate with Auth service for Authentication and Authorization</t>
+  </si>
+  <si>
+    <t>Integrate with Auth service to get permissions, and implement Ocelot's middleware to handle restricted permission. Need to implement for own handling instead of using default Ocelot configuration</t>
+  </si>
+  <si>
+    <t>SCRUM-49</t>
+  </si>
+  <si>
+    <t>Implement Auth Service</t>
+  </si>
+  <si>
+    <t>Migrate Authentication and Authorization from User service</t>
+  </si>
+  <si>
+    <t>Implement API to get permission for user</t>
+  </si>
+  <si>
+    <t>Implement UAM for database design</t>
+  </si>
+  <si>
+    <t>Implement the basic Ocelot service within some basic configuration to forward requests only</t>
+  </si>
+  <si>
+    <t>SCRUM-51</t>
+  </si>
+  <si>
+    <t>SCRUM-52</t>
+  </si>
+  <si>
+    <t>SCRUM-53</t>
+  </si>
+  <si>
+    <t>Migrate and implement the auth service to handle login and internal login, exchange tokens from User service</t>
+  </si>
+  <si>
+    <t>Design the database to implement UAM to be able to integrate with the Ocelot service</t>
+  </si>
+  <si>
+    <t>FB001-31</t>
+  </si>
+  <si>
+    <t>FB001-44</t>
+  </si>
+  <si>
+    <t>FB001-50</t>
+  </si>
+  <si>
+    <t>Implement Auth Service for mainly provide the API for Ocelot service to perform Authentication and Authorization</t>
+  </si>
+  <si>
+    <t>Implement IdP Server for Internal User Authentication</t>
   </si>
 </sst>
 </file>
@@ -651,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,6 +822,27 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -784,33 +882,39 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -819,12 +923,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1311,7 +1409,7 @@
   <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1366,26 +1464,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="11"/>
+    <row r="6" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
@@ -1432,12 +1542,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1460,13 +1570,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="46" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1480,9 +1590,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1494,9 +1604,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1536,13 +1646,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="49" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1556,9 +1666,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1570,13 +1680,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="42" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1590,9 +1700,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1714,7 +1824,7 @@
   <dimension ref="A2:F29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,12 +1839,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1760,10 +1870,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="50" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1778,8 +1888,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1792,8 +1902,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1806,8 +1916,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -1820,8 +1930,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -1947,13 +2057,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="54" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -1967,9 +2077,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -1981,9 +2091,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2091,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B875EC8-ACE7-474A-B26E-31D1589A2243}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2107,12 +2217,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2135,13 +2245,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="50" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2155,9 +2265,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2169,9 +2279,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2183,13 +2293,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="64" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2203,9 +2313,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="56"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2217,9 +2327,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="57"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2362,4 +2472,472 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FCE00F-CF72-8643-96EF-AADFC0D8B388}">
+  <dimension ref="A2:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="57.5" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="74.83203125" customWidth="1"/>
+    <col min="6" max="6" width="80.5" customWidth="1"/>
+    <col min="7" max="9" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A6" s="56"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A7" s="57"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A9" s="59"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297FA735-DC77-0149-8CB1-2DDFFD73CB7C}">
+  <dimension ref="A2:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="57.5" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="74.83203125" customWidth="1"/>
+    <col min="6" max="6" width="80.5" customWidth="1"/>
+    <col min="7" max="9" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FB001-48: Containerize the Ocelot Server application
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5074F2-E380-EB4B-9DF1-71461067B484}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789374C-8FA5-BA4E-82AC-42AB2F1FB9C1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="4" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="156">
   <si>
     <t>Description</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>Implement IdP Server for Internal User Authentication</t>
+  </si>
+  <si>
+    <t>Containerize the Ocelot Server application</t>
+  </si>
+  <si>
+    <t>Create CI/CD to deploy Ocelot to Cluster for two environments</t>
   </si>
 </sst>
 </file>
@@ -2479,7 +2485,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2549,10 +2555,10 @@
         <v>134</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
@@ -2563,10 +2569,10 @@
         <v>138</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -2738,7 +2744,7 @@
   <dimension ref="A2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
FB001-54: Create Auth service and migrate User service APIs
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789374C-8FA5-BA4E-82AC-42AB2F1FB9C1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64A09E2-8C77-8543-8963-E00DE6B89859}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="4" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="5" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="166">
   <si>
     <t>Description</t>
   </si>
@@ -503,6 +503,36 @@
   </si>
   <si>
     <t>Create CI/CD to deploy Ocelot to Cluster for two environments</t>
+  </si>
+  <si>
+    <t>SCRUM-54</t>
+  </si>
+  <si>
+    <t>Create Auth service and migrate User service APIs</t>
+  </si>
+  <si>
+    <t>Create Auth service and migrate necessary User service APIs to this service for clear responsibility</t>
+  </si>
+  <si>
+    <t>SCRUM-55</t>
+  </si>
+  <si>
+    <t>SCRUM-56</t>
+  </si>
+  <si>
+    <t>Containerize the Auth Service application</t>
+  </si>
+  <si>
+    <t>Create CI/CD to deploy Auth service to Cluster for two environments</t>
+  </si>
+  <si>
+    <t>SCRUM-57</t>
+  </si>
+  <si>
+    <t>Correct API Endpoints after migrating new service</t>
+  </si>
+  <si>
+    <t>Correct API Endpoints after migrating new service, UI can work with new services</t>
   </si>
 </sst>
 </file>
@@ -734,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -847,6 +877,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1548,12 +1587,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1576,13 +1615,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="49" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1596,9 +1635,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1610,9 +1649,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1652,13 +1691,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="52" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1672,9 +1711,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1686,13 +1725,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="45" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1706,9 +1745,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1845,12 +1884,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1876,10 +1915,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="53" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1894,8 +1933,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1908,8 +1947,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1922,8 +1961,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -1936,8 +1975,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2063,13 +2102,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="57" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2083,9 +2122,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="53"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -2097,9 +2136,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="53"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2223,12 +2262,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2251,13 +2290,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="53" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2271,9 +2310,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="56"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2285,9 +2324,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2299,13 +2338,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="67" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2319,9 +2358,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="65"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2333,9 +2372,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="66"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2484,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FCE00F-CF72-8643-96EF-AADFC0D8B388}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2500,12 +2539,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2528,13 +2567,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="53" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2548,9 +2587,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="56"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2562,9 +2601,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="20" t="s">
         <v>138</v>
       </c>
@@ -2576,13 +2615,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="67" t="s">
         <v>137</v>
       </c>
       <c r="D8" s="39"/>
@@ -2590,17 +2629,17 @@
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="65"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="39"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="66"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="39"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -2741,10 +2780,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297FA735-DC77-0149-8CB1-2DDFFD73CB7C}">
-  <dimension ref="A2:F21"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2752,19 +2791,19 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="57.5" customWidth="1"/>
     <col min="3" max="3" width="98" customWidth="1"/>
-    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="74.83203125" customWidth="1"/>
     <col min="6" max="6" width="80.5" customWidth="1"/>
     <col min="7" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2796,77 +2835,101 @@
       <c r="C5" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="D5" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="42"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A7" s="42"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A8" s="42"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B9" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C9" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B10" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C10" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+    </row>
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A11" s="39"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
@@ -2933,12 +2996,36 @@
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
FB001-55: Containerize the Auth Service application
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64A09E2-8C77-8543-8963-E00DE6B89859}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B7FBEA-DA27-344D-A0BB-86FC4D6D8B83}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1140" windowWidth="37820" windowHeight="19660" activeTab="5" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="580" yWindow="1180" windowWidth="37820" windowHeight="19660" activeTab="5" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="168">
   <si>
     <t>Description</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>Correct API Endpoints after migrating new service, UI can work with new services</t>
+  </si>
+  <si>
+    <t>SCRUM-58</t>
+  </si>
+  <si>
+    <t>Sync User data after api register is executed</t>
   </si>
 </sst>
 </file>
@@ -2783,7 +2789,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2915,10 +2921,16 @@
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
     </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+    <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>167</v>
+      </c>
       <c r="D11" s="35"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>

</xml_diff>

<commit_message>
FB001-60: [User Service] Change to use MySQL to replace SQL Server
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B7FBEA-DA27-344D-A0BB-86FC4D6D8B83}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD284D5-D49D-4F47-BE61-D1DC30CBE6F6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1180" windowWidth="37820" windowHeight="19660" activeTab="5" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="173">
   <si>
     <t>Description</t>
   </si>
@@ -539,6 +539,21 @@
   </si>
   <si>
     <t>Sync User data after api register is executed</t>
+  </si>
+  <si>
+    <t>SCRUM-60</t>
+  </si>
+  <si>
+    <t>[User Service] Change to use MySQL to replace SQL Server</t>
+  </si>
+  <si>
+    <t>Change to use MySQL to replace SQL Server, because of the memory usage problem</t>
+  </si>
+  <si>
+    <t>SCRUM-61</t>
+  </si>
+  <si>
+    <t>[Cluster] Upgrade RAM, CPU for Cluster Nodes</t>
   </si>
 </sst>
 </file>
@@ -770,7 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -892,6 +907,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1593,12 +1614,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1621,13 +1642,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="51" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1641,9 +1662,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1655,9 +1676,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1697,13 +1718,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="54" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1717,9 +1738,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1731,13 +1752,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="47" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1751,9 +1772,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1890,12 +1911,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1921,10 +1942,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="55" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1939,8 +1960,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1953,8 +1974,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1967,8 +1988,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -1981,8 +2002,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2108,13 +2129,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="59" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2128,9 +2149,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="56"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -2142,9 +2163,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="56"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2268,12 +2289,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2296,13 +2317,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="55" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2316,9 +2337,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="59"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2330,9 +2351,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2344,13 +2365,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="69" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2364,9 +2385,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="68"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2378,9 +2399,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="69"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2545,12 +2566,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2573,13 +2594,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="55" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2593,9 +2614,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="59"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2607,9 +2628,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="20" t="s">
         <v>138</v>
       </c>
@@ -2621,13 +2642,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="69" t="s">
         <v>137</v>
       </c>
       <c r="D8" s="39"/>
@@ -2635,17 +2656,17 @@
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="68"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="39"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="69"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="39"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -2789,7 +2810,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2804,12 +2825,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2935,21 +2956,33 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+    </row>
+    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A13" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>

</xml_diff>

<commit_message>
FB001-63: Implement Middleware to handle Authentication and Authorization
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD284D5-D49D-4F47-BE61-D1DC30CBE6F6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F51F386-7248-9345-B5A7-7F2BE80C1437}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1180" windowWidth="37820" windowHeight="19660" activeTab="5" xr2:uid="{14631E72-EE2B-0947-82C4-7D9E8B7B85EF}"/>
+    <workbookView xWindow="580" yWindow="1180" windowWidth="37820" windowHeight="19660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="177">
   <si>
     <t>Description</t>
   </si>
@@ -554,6 +554,18 @@
   </si>
   <si>
     <t>[Cluster] Upgrade RAM, CPU for Cluster Nodes</t>
+  </si>
+  <si>
+    <t>Implement Middleware to handle Authentication and Authorization</t>
+  </si>
+  <si>
+    <t>SCRUM-63</t>
+  </si>
+  <si>
+    <t>Implement the common Error-handling Middleware for BE</t>
+  </si>
+  <si>
+    <t>SCRUM-64</t>
   </si>
 </sst>
 </file>
@@ -785,7 +797,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -882,119 +894,128 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1016,7 +1037,6 @@
         <sz val="18"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1047,7 +1067,6 @@
         <sz val="18"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1082,7 +1101,6 @@
         <sz val="18"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1145,7 +1163,6 @@
         <sz val="18"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1170,12 +1187,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9943E95-7229-7E48-8A2C-EB277E640B62}" name="Table2" displayName="Table2" ref="A2:C10" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A2:C10" xr:uid="{804D9C77-02EF-5748-9F9F-BA92FEF1283F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:C10" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A2:C10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1A8BFCAF-6BBD-1248-B600-DC87C79B6A4A}" name="Epic Id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{3BB16C9F-86E6-1D44-AEAB-7CD6882748DB}" name="Epic Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{C9482C12-6566-EF42-A811-D0886FFB8A2C}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Epic Id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Epic Name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1477,14 +1494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D1A78A-886E-1049-9493-3E3336989B94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="89.33203125" style="9" customWidth="1"/>
@@ -1585,7 +1602,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="SCRUM-1" xr:uid="{BD44C65E-8536-A141-803F-7CE5EE80C51F}"/>
+    <hyperlink ref="A3" r:id="rId1" display="SCRUM-1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1595,14 +1612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71808AEC-1F3F-6046-97A2-6661A8254E1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="61.5" customWidth="1"/>
@@ -1614,12 +1631,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1642,13 +1659,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="53" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1662,9 +1679,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1676,9 +1693,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1718,13 +1735,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="55" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1738,9 +1755,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1752,13 +1769,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="49" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1772,9 +1789,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1785,13 +1802,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+    <row r="14" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
@@ -1892,14 +1915,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5C440-AD56-C140-BA37-3A80F9AAE5E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:F29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="61.5" customWidth="1"/>
@@ -1911,12 +1934,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1942,10 +1965,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1960,8 +1983,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1974,8 +1997,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -1988,8 +2011,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -2002,8 +2025,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2129,13 +2152,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="60" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2149,9 +2172,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -2163,9 +2186,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2270,14 +2293,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B875EC8-ACE7-474A-B26E-31D1589A2243}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="61.5" customWidth="1"/>
@@ -2289,12 +2312,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2317,13 +2340,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2337,9 +2360,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2351,9 +2374,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="62"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2365,13 +2388,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="70" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2385,9 +2408,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2399,9 +2422,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="71"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2547,14 +2570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FCE00F-CF72-8643-96EF-AADFC0D8B388}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="D6" sqref="D6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="57.5" customWidth="1"/>
@@ -2566,12 +2589,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2594,13 +2617,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2614,9 +2637,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2628,9 +2651,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="62"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="20" t="s">
         <v>138</v>
       </c>
@@ -2642,32 +2665,32 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="39"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="39"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
@@ -2675,15 +2698,15 @@
       <c r="A11" s="20"/>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
-      <c r="D11" s="37"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="35"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
@@ -2806,14 +2829,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297FA735-DC77-0149-8CB1-2DDFFD73CB7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="57.5" customWidth="1"/>
@@ -2825,12 +2848,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2853,83 +2876,83 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="40" t="s">
         <v>156</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="39" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="39" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>146</v>
       </c>
       <c r="B10" s="33" t="s">
@@ -2938,12 +2961,18 @@
       <c r="C10" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
+      <c r="D10" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="38" t="s">
         <v>166</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -2952,7 +2981,7 @@
       <c r="C11" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
@@ -2960,18 +2989,18 @@
       <c r="A12" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>170</v>
       </c>
       <c r="D12" s="20"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="42" t="s">
         <v>171</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -2980,7 +3009,7 @@
       <c r="C13" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="44"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
@@ -3073,8 +3102,11 @@
       <c r="F24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FB001-66: Using Openssl to generate private/public key
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F51F386-7248-9345-B5A7-7F2BE80C1437}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB46D9-EC96-0740-A5B6-88E4CFE4D0C5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1180" windowWidth="37820" windowHeight="19660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="1740" windowWidth="35860" windowHeight="19100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="185">
   <si>
     <t>Description</t>
   </si>
@@ -566,6 +566,30 @@
   </si>
   <si>
     <t>SCRUM-64</t>
+  </si>
+  <si>
+    <t>Update Exchange token API</t>
+  </si>
+  <si>
+    <t>SCRUM-65</t>
+  </si>
+  <si>
+    <t>Using Openssl to generate private/public key</t>
+  </si>
+  <si>
+    <t>Validate IdP Token on Auth service</t>
+  </si>
+  <si>
+    <t>Generate IdP Token by Private key for IdP Service</t>
+  </si>
+  <si>
+    <t>SCRUM-66</t>
+  </si>
+  <si>
+    <t>SCRUM-67</t>
+  </si>
+  <si>
+    <t>SCRUM-68</t>
   </si>
 </sst>
 </file>
@@ -797,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -933,6 +957,12 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -957,6 +987,12 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1010,12 +1046,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1615,7 +1645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C10" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
@@ -1631,12 +1661,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1659,13 +1689,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="55" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1679,9 +1709,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1693,9 +1723,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="54"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1735,13 +1765,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="59" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1755,9 +1785,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="74"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1769,13 +1799,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="51" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1789,9 +1819,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1934,12 +1964,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1965,10 +1995,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="60" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1983,8 +2013,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -1997,8 +2027,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -2011,8 +2041,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -2025,8 +2055,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2152,13 +2182,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="64" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2172,9 +2202,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="59"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -2186,9 +2216,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="59"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2312,12 +2342,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2340,13 +2370,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="60" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2360,9 +2390,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2374,9 +2404,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2388,13 +2418,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="74" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2408,9 +2438,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="71"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2422,9 +2452,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="72"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2589,12 +2619,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2617,13 +2647,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="60" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="60" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2637,9 +2667,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2651,9 +2681,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
         <v>138</v>
       </c>
@@ -2665,13 +2695,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="74" t="s">
         <v>137</v>
       </c>
       <c r="D8" s="38"/>
@@ -2679,17 +2709,17 @@
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="71"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="38"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="72"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="38"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -2832,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2848,12 +2878,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2876,13 +2906,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="60" t="s">
         <v>147</v>
       </c>
       <c r="D5" s="40" t="s">
@@ -2896,9 +2926,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="20" t="s">
         <v>159</v>
       </c>
@@ -2910,9 +2940,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="62"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20" t="s">
         <v>160</v>
       </c>
@@ -2924,9 +2954,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="20" t="s">
         <v>163</v>
       </c>
@@ -3013,29 +3043,53 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+    <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>

</xml_diff>

<commit_message>
FB001-67: Generate IdP Token by Private key for IdP Service
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB46D9-EC96-0740-A5B6-88E4CFE4D0C5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831ADC5-5809-D648-BCC8-4ECB1961978D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1740" windowWidth="35860" windowHeight="19100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="189">
   <si>
     <t>Description</t>
   </si>
@@ -538,9 +538,6 @@
     <t>SCRUM-58</t>
   </si>
   <si>
-    <t>Sync User data after api register is executed</t>
-  </si>
-  <si>
     <t>SCRUM-60</t>
   </si>
   <si>
@@ -590,6 +587,21 @@
   </si>
   <si>
     <t>SCRUM-68</t>
+  </si>
+  <si>
+    <t>Design database for IdP service</t>
+  </si>
+  <si>
+    <t>SCRUM-69</t>
+  </si>
+  <si>
+    <t>Design database service</t>
+  </si>
+  <si>
+    <t>SCRUM-70</t>
+  </si>
+  <si>
+    <t>Sync User data after api register/exchange token is executed</t>
   </si>
 </sst>
 </file>
@@ -821,7 +833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -963,6 +975,9 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1045,6 +1060,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1661,12 +1685,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1689,13 +1713,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1709,9 +1733,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="56"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1723,9 +1747,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="56"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1765,13 +1789,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="60" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1785,9 +1809,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1799,13 +1823,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="52" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1819,9 +1843,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="50"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1834,13 +1858,13 @@
     </row>
     <row r="14" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="45"/>
@@ -1964,12 +1988,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1995,10 +2019,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="61" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2013,8 +2037,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -2027,8 +2051,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -2041,8 +2065,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -2055,8 +2079,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2182,13 +2206,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="65" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2202,9 +2226,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -2216,9 +2240,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2342,12 +2366,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2370,13 +2394,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="61" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2390,9 +2414,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2404,9 +2428,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2418,13 +2442,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="75" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2438,9 +2462,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="75"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2452,9 +2476,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="70"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="76"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2619,12 +2643,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2647,13 +2671,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="61" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2667,9 +2691,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2681,9 +2705,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="20" t="s">
         <v>138</v>
       </c>
@@ -2695,13 +2719,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="75" t="s">
         <v>137</v>
       </c>
       <c r="D8" s="38"/>
@@ -2709,17 +2733,17 @@
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="75"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="38"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="70"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="76"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="38"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -2863,7 +2887,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2878,12 +2902,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2906,13 +2930,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="66" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="61" t="s">
         <v>147</v>
       </c>
       <c r="D5" s="40" t="s">
@@ -2926,9 +2950,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="20" t="s">
         <v>159</v>
       </c>
@@ -2940,9 +2964,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="20" t="s">
         <v>160</v>
       </c>
@@ -2954,9 +2978,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="20" t="s">
         <v>163</v>
       </c>
@@ -2992,24 +3016,24 @@
         <v>148</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>166</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="22"/>
@@ -3017,13 +3041,13 @@
     </row>
     <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="C12" s="41" t="s">
         <v>169</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>170</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="41"/>
@@ -3031,89 +3055,101 @@
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>172</v>
-      </c>
       <c r="C13" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13" s="42"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" s="20" t="s">
+      <c r="F14" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A15" s="67"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E15" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A16" s="68"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F16" s="48" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="20" t="s">
+    <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A17" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="C17" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
@@ -3156,11 +3192,14 @@
       <c r="F24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FB001-71: [IdP Service]Create Internal API to get User details without authentication
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831ADC5-5809-D648-BCC8-4ECB1961978D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F666295-99B0-2B44-85A4-817548E30441}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1740" windowWidth="35860" windowHeight="19100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="1920" windowWidth="35860" windowHeight="19100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="196">
   <si>
     <t>Description</t>
   </si>
@@ -602,6 +602,27 @@
   </si>
   <si>
     <t>Sync User data after api register/exchange token is executed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[IdP Service]Create Internal API to get User details without authentication </t>
+  </si>
+  <si>
+    <t>Implement the solution to authenticate for internal API, Create the core implementation to handle common calling Internal API Service</t>
+  </si>
+  <si>
+    <t>SCRUM-72</t>
+  </si>
+  <si>
+    <t>Create a Library for Internal Synchronous API Service</t>
+  </si>
+  <si>
+    <t>Create a Library for Internal Asynchronous API Service</t>
+  </si>
+  <si>
+    <t>Implement message broker, create the core implementation to handle common consuming API</t>
+  </si>
+  <si>
+    <t>SCRUM-73</t>
   </si>
 </sst>
 </file>
@@ -833,7 +854,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -973,6 +994,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1669,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,12 +1721,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1713,13 +1749,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="125" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="61" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1733,9 +1769,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1747,9 +1783,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1789,13 +1825,13 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="65" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1809,9 +1845,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1823,13 +1859,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="57" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1843,9 +1879,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1870,21 +1906,33 @@
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
     </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+    <row r="15" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A15" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+    </row>
+    <row r="16" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A16" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
@@ -1988,12 +2036,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2019,10 +2067,10 @@
       <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="66" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2037,8 +2085,8 @@
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="20" t="s">
         <v>85</v>
       </c>
@@ -2051,8 +2099,8 @@
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
@@ -2065,8 +2113,8 @@
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="20" t="s">
         <v>80</v>
       </c>
@@ -2079,8 +2127,8 @@
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2206,13 +2254,13 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="70" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2226,9 +2274,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A18" s="64"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="32" t="s">
         <v>122</v>
       </c>
@@ -2240,9 +2288,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A19" s="64"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="32" t="s">
         <v>126</v>
       </c>
@@ -2366,12 +2414,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2394,13 +2442,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="66" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2414,9 +2462,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="20" t="s">
         <v>104</v>
       </c>
@@ -2428,9 +2476,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="68"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="20" t="s">
         <v>105</v>
       </c>
@@ -2442,13 +2490,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="80" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2462,9 +2510,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="76"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
@@ -2476,9 +2524,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="77"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="21" t="s">
         <v>108</v>
       </c>
@@ -2643,12 +2691,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2671,13 +2719,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="66" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2691,9 +2739,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2705,9 +2753,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="68"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="20" t="s">
         <v>138</v>
       </c>
@@ -2719,13 +2767,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="80" t="s">
         <v>137</v>
       </c>
       <c r="D8" s="38"/>
@@ -2733,17 +2781,17 @@
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="76"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="38"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="77"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="38"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -2884,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2902,12 +2950,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2930,13 +2978,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="66" t="s">
         <v>147</v>
       </c>
       <c r="D5" s="40" t="s">
@@ -2950,9 +2998,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="20" t="s">
         <v>159</v>
       </c>
@@ -2964,9 +3012,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="20" t="s">
         <v>160</v>
       </c>
@@ -2978,9 +3026,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A8" s="68"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="20" t="s">
         <v>163</v>
       </c>
@@ -3068,13 +3116,13 @@
       <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="83" t="s">
         <v>176</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -3088,9 +3136,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A15" s="67"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="20" t="s">
         <v>182</v>
       </c>
@@ -3102,9 +3150,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A16" s="68"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="84"/>
       <c r="D16" s="20" t="s">
         <v>183</v>
       </c>
@@ -3115,33 +3163,39 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A17" s="73"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B18" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C18" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D18" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E18" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F18" s="22" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
@@ -3151,13 +3205,13 @@
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
     </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
@@ -3184,12 +3238,20 @@
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3197,9 +3259,9 @@
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FB001-79: Create pipeline feature and integrate with .Net API server and Jenkins
</commit_message>
<xml_diff>
--- a/Documents/ManageTasks.xlsx
+++ b/Documents/ManageTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huynhngocson/Desktop/up-skills/Fakebook/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F666295-99B0-2B44-85A4-817548E30441}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C52E9-6BC4-6A44-92B5-5BF9A8BEDE78}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1920" windowWidth="35860" windowHeight="19100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="1920" windowWidth="35860" windowHeight="19100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="FB001-31" sheetId="5" r:id="rId4"/>
     <sheet name="FB001-44" sheetId="6" r:id="rId5"/>
     <sheet name="FB001-50" sheetId="7" r:id="rId6"/>
+    <sheet name="FB001-83" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="245">
   <si>
     <t>Description</t>
   </si>
@@ -623,6 +624,153 @@
   </si>
   <si>
     <t>SCRUM-73</t>
+  </si>
+  <si>
+    <t>Implement Post Service</t>
+  </si>
+  <si>
+    <t>Create the first Post Service</t>
+  </si>
+  <si>
+    <t>Create the API server for Post service</t>
+  </si>
+  <si>
+    <t>FB001-83</t>
+  </si>
+  <si>
+    <t>Implement Post Service for mainly provide API to interact with user Posts</t>
+  </si>
+  <si>
+    <t>Design the database for Post service</t>
+  </si>
+  <si>
+    <t>Design databases to handle Post, Like, Comment, Share</t>
+  </si>
+  <si>
+    <t>Create API to CRUD Post</t>
+  </si>
+  <si>
+    <t>Create API to create comment for Post/Comment</t>
+  </si>
+  <si>
+    <t>Create API to Like/Unlike post/comment</t>
+  </si>
+  <si>
+    <t>Create API to create comment for Post/Comment by level</t>
+  </si>
+  <si>
+    <t>Containerize the Post API Server application</t>
+  </si>
+  <si>
+    <t>Create CI/CD to deploy Post API to Cluster for two environments</t>
+  </si>
+  <si>
+    <t>Implement the Notification Service</t>
+  </si>
+  <si>
+    <t>Create Real Time Notification Service</t>
+  </si>
+  <si>
+    <t>Create the Feed Component</t>
+  </si>
+  <si>
+    <t>Create the Feed Component to load all the Posts related to logged-in User</t>
+  </si>
+  <si>
+    <t>Create Post Detail Component</t>
+  </si>
+  <si>
+    <t>Create Post Detail Component for single Post</t>
+  </si>
+  <si>
+    <t>Create Comment Component</t>
+  </si>
+  <si>
+    <t>Create Comment Component by level, which can be comment for Post or another comment</t>
+  </si>
+  <si>
+    <t>Create Like/Comment/Share control component</t>
+  </si>
+  <si>
+    <t>Create Feed Component</t>
+  </si>
+  <si>
+    <t>Create Feed Component to render all of the Posts/Likes/Comments</t>
+  </si>
+  <si>
+    <t>Create the Template for Logged-In user Home Page</t>
+  </si>
+  <si>
+    <t>Create the Template for Logged-In user Home Page, which is copied from available template</t>
+  </si>
+  <si>
+    <t>SCRUM-84</t>
+  </si>
+  <si>
+    <t>SCRUM-85</t>
+  </si>
+  <si>
+    <t>SCRUM-86</t>
+  </si>
+  <si>
+    <t>SCRUM-87</t>
+  </si>
+  <si>
+    <t>SCRUM-88</t>
+  </si>
+  <si>
+    <t>SCRUM-89</t>
+  </si>
+  <si>
+    <t>SCRUM-90</t>
+  </si>
+  <si>
+    <t>SCRUM-91</t>
+  </si>
+  <si>
+    <t>SCRUM-92</t>
+  </si>
+  <si>
+    <t>SCRUM-93</t>
+  </si>
+  <si>
+    <t>SCRUM-94</t>
+  </si>
+  <si>
+    <t>SCRUM-95</t>
+  </si>
+  <si>
+    <t>SCRUM-96</t>
+  </si>
+  <si>
+    <t>SCRUM-97</t>
+  </si>
+  <si>
+    <t>SCRUM-98</t>
+  </si>
+  <si>
+    <t>SCRUM-99</t>
+  </si>
+  <si>
+    <t>SCRUM-100</t>
+  </si>
+  <si>
+    <t>SCRUM-101</t>
+  </si>
+  <si>
+    <t>SCRUM-102</t>
+  </si>
+  <si>
+    <t>SCRUM-103</t>
+  </si>
+  <si>
+    <t>Notify for the Online user when one user creates the Post</t>
+  </si>
+  <si>
+    <t>Notify for the Online user when one user creates the Post in public mode</t>
+  </si>
+  <si>
+    <t>Notify the User when they first log in when one user creates the Post with public mode</t>
   </si>
 </sst>
 </file>
@@ -741,7 +889,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -785,17 +933,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -854,7 +991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -869,22 +1006,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -924,187 +1058,196 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1261,8 +1404,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFF2CC"/>
       <color rgb="FFDDEBF7"/>
-      <color rgb="FFFFF2CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1588,14 +1731,14 @@
   <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="89.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="148.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="89.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="148.5" style="8" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1611,84 +1754,88 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="62" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="50" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="11"/>
+    <row r="9" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1705,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,22 +1876,22 @@
       <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1758,13 +1905,13 @@
       <c r="C5" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1772,13 +1919,13 @@
       <c r="A6" s="62"/>
       <c r="B6" s="60"/>
       <c r="C6" s="61"/>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1786,43 +1933,43 @@
       <c r="A7" s="62"/>
       <c r="B7" s="60"/>
       <c r="C7" s="61"/>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
       <c r="A10" s="63" t="s">
@@ -1834,13 +1981,13 @@
       <c r="C10" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1848,13 +1995,13 @@
       <c r="A11" s="64"/>
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1868,13 +2015,13 @@
       <c r="C12" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1882,113 +2029,113 @@
       <c r="A13" s="56"/>
       <c r="B13" s="58"/>
       <c r="C13" s="58"/>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
@@ -2021,7 +2168,7 @@
   <dimension ref="A2:F29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2044,27 +2191,27 @@
       <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="71" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="66" t="s">
@@ -2073,185 +2220,185 @@
       <c r="C5" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="100" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="67"/>
       <c r="C7" s="67"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67"/>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="27" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="100" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="20" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A17" s="69" t="s">
@@ -2263,13 +2410,13 @@
       <c r="C17" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="21" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2277,13 +2424,13 @@
       <c r="A18" s="69"/>
       <c r="B18" s="70"/>
       <c r="C18" s="70"/>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="21" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2291,87 +2438,87 @@
       <c r="A19" s="69"/>
       <c r="B19" s="70"/>
       <c r="C19" s="70"/>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="21" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
@@ -2382,13 +2529,14 @@
       <c r="F29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A5:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2399,7 +2547,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="E6" sqref="E6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2422,22 +2570,22 @@
       <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2451,13 +2599,13 @@
       <c r="C5" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="29" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2465,13 +2613,13 @@
       <c r="A6" s="72"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="29" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2479,13 +2627,13 @@
       <c r="A7" s="73"/>
       <c r="B7" s="67"/>
       <c r="C7" s="67"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="29" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2499,13 +2647,13 @@
       <c r="C8" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2513,13 +2661,13 @@
       <c r="A9" s="75"/>
       <c r="B9" s="78"/>
       <c r="C9" s="81"/>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2527,127 +2675,127 @@
       <c r="A10" s="76"/>
       <c r="B10" s="79"/>
       <c r="C10" s="82"/>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
@@ -2676,7 +2824,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2699,22 +2847,22 @@
       <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2728,13 +2876,13 @@
       <c r="C5" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="31" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2742,13 +2890,13 @@
       <c r="A6" s="72"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="31" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2756,13 +2904,13 @@
       <c r="A7" s="73"/>
       <c r="B7" s="67"/>
       <c r="C7" s="67"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="31" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2776,137 +2924,137 @@
       <c r="C8" s="80" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="78"/>
       <c r="C9" s="81"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="76"/>
       <c r="B10" s="79"/>
       <c r="C10" s="82"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
@@ -2935,7 +3083,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2958,22 +3106,22 @@
       <c r="E2" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2987,13 +3135,13 @@
       <c r="C5" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="37" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3001,13 +3149,13 @@
       <c r="A6" s="72"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="37" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3015,13 +3163,13 @@
       <c r="A7" s="72"/>
       <c r="B7" s="67"/>
       <c r="C7" s="67"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="37" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3029,91 +3177,91 @@
       <c r="A8" s="73"/>
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="37" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="41" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
       <c r="A14" s="71" t="s">
@@ -3125,13 +3273,13 @@
       <c r="C14" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="46" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3139,13 +3287,13 @@
       <c r="A15" s="72"/>
       <c r="B15" s="67"/>
       <c r="C15" s="84"/>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="46" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3153,13 +3301,13 @@
       <c r="A16" s="72"/>
       <c r="B16" s="67"/>
       <c r="C16" s="84"/>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="46" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3167,83 +3315,83 @@
       <c r="A17" s="73"/>
       <c r="B17" s="68"/>
       <c r="C17" s="85"/>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="F17" s="50" t="s">
+      <c r="F17" s="48" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="21" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
@@ -3265,4 +3413,404 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E2781D-219F-6643-BD5B-347DBB228387}">
+  <dimension ref="A2:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="57.5" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="74.83203125" customWidth="1"/>
+    <col min="6" max="6" width="80.5" customWidth="1"/>
+    <col min="7" max="9" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+    </row>
+    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A5" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A6" s="86"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A7" s="86"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A8" s="86"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A9" s="86"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A10" s="86"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A11" s="86"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A12" s="69" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="87" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A13" s="69"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A14" s="69"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A15" s="69"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A16" s="69"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A17" s="86" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A18" s="86"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A19" s="86"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+      <c r="A20" s="86"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="50" x14ac:dyDescent="0.2">
+      <c r="A21" s="86"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="C5:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>